<commit_message>
Icon changed to Grand Piano
</commit_message>
<xml_diff>
--- a/View/Images/_Image Sources.xlsx
+++ b/View/Images/_Image Sources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\OneDrive\Documents\Visual Studio Projects\SoundExplorers\Archivists' App\View\Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\OneDrive\Documents\Visual Studio Projects\SoundExplorers\View\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965F969D-8297-4D6D-94DB-75D1C1215BA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0301CA-9614-47BC-8F10-ACF140F8BCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{185F787C-75CB-4C6E-8AE2-88ADA4650E2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Cut Flatastic 32x32</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Link Webuosities 32x32</t>
+  </si>
+  <si>
+    <t>Grand Piano</t>
+  </si>
+  <si>
+    <t>https://www.iconshock.com/musical-instruments-icons/</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B372047D-F86E-4F80-A455-C4F35445834D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -490,6 +496,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{350207DB-0925-4306-86A0-D41A784B49BD}"/>
@@ -498,6 +512,7 @@
     <hyperlink ref="B6" r:id="rId4" xr:uid="{E2141F60-C2D4-49D8-8715-15947578773F}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{86757DA5-FD61-406E-9E9C-B8732EC2C704}"/>
     <hyperlink ref="B5" r:id="rId6" xr:uid="{7BD57134-0B66-4797-9CAD-1BC290707EB2}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{60BC7BDE-69E2-4C5B-8686-00278A6549F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed icon to kettle drum. Copy system database files to database folder if required. Added version to installer title.
</commit_message>
<xml_diff>
--- a/View/Images/_Image Sources.xlsx
+++ b/View/Images/_Image Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\OneDrive\Documents\Visual Studio Projects\SoundExplorers\View\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0301CA-9614-47BC-8F10-ACF140F8BCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817E5B52-96E4-45E2-A36F-AE5C71357E89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{185F787C-75CB-4C6E-8AE2-88ADA4650E2D}"/>
+    <workbookView xWindow="2568" yWindow="3180" windowWidth="17280" windowHeight="10044" xr2:uid="{185F787C-75CB-4C6E-8AE2-88ADA4650E2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Cut Flatastic 32x32</t>
   </si>
@@ -72,10 +72,13 @@
     <t>Link Webuosities 32x32</t>
   </si>
   <si>
+    <t>https://www.iconshock.com/musical-instruments-icons/</t>
+  </si>
+  <si>
+    <t>Kettle Drum</t>
+  </si>
+  <si>
     <t>Grand Piano</t>
-  </si>
-  <si>
-    <t>https://www.iconshock.com/musical-instruments-icons/</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B372047D-F86E-4F80-A455-C4F35445834D}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -498,10 +501,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -513,6 +524,7 @@
     <hyperlink ref="B4" r:id="rId5" xr:uid="{86757DA5-FD61-406E-9E9C-B8732EC2C704}"/>
     <hyperlink ref="B5" r:id="rId6" xr:uid="{7BD57134-0B66-4797-9CAD-1BC290707EB2}"/>
     <hyperlink ref="B7" r:id="rId7" xr:uid="{60BC7BDE-69E2-4C5B-8686-00278A6549F8}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{F2577189-4D64-44E2-BD27-0ACA9F0CA0E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>